<commit_message>
Replaced the stringly-typed Effect will a proper class heirarchy.
</commit_message>
<xml_diff>
--- a/7W/Resources/cardText/7 Wonders Card list.xlsx
+++ b/7W/Resources/cardText/7 Wonders Card list.xlsx
@@ -5,18 +5,19 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\7-Wonders-Leaders\7W\Resources\cardText\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\7-Wonders-Leaders\7W\Resources\cardText\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="31110" windowHeight="15420"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="31110" windowHeight="15420" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Mine" sheetId="1" r:id="rId1"/>
-    <sheet name="Existing game" sheetId="2" r:id="rId2"/>
+    <sheet name="Cards" sheetId="1" r:id="rId1"/>
+    <sheet name="Wonders" sheetId="3" r:id="rId2"/>
+    <sheet name="Existing game" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Mine!$A$1:$AD$80</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Cards!$A$1:$AD$80</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="340">
   <si>
     <t>Age</t>
   </si>
@@ -354,18 +355,6 @@
     <t>Path</t>
   </si>
   <si>
-    <t>Blue</t>
-  </si>
-  <si>
-    <t>12V</t>
-  </si>
-  <si>
-    <t>Not used</t>
-  </si>
-  <si>
-    <t>! (Free)</t>
-  </si>
-  <si>
     <t>Categories</t>
   </si>
   <si>
@@ -381,9 +370,6 @@
     <t>one of a kind cards, except science</t>
   </si>
   <si>
-    <t>2 victory points to the holder's city</t>
-  </si>
-  <si>
     <t>Cards which require the player to make a choice between resources</t>
   </si>
   <si>
@@ -853,6 +839,216 @@
   </si>
   <si>
     <t>gear</t>
+  </si>
+  <si>
+    <t>Simple</t>
+  </si>
+  <si>
+    <t>ResourceChoice</t>
+  </si>
+  <si>
+    <t>CoinsPoints</t>
+  </si>
+  <si>
+    <t>SpecializedGuild</t>
+  </si>
+  <si>
+    <t>Alexandria (A)</t>
+  </si>
+  <si>
+    <t>Starting Resource</t>
+  </si>
+  <si>
+    <t>Stages</t>
+  </si>
+  <si>
+    <t>Stage 1 cost</t>
+  </si>
+  <si>
+    <t>TT</t>
+  </si>
+  <si>
+    <t>Stage 1 effect</t>
+  </si>
+  <si>
+    <t>13V</t>
+  </si>
+  <si>
+    <t>Stage 2 cost</t>
+  </si>
+  <si>
+    <t>Stage 2 effect</t>
+  </si>
+  <si>
+    <t>Stage 3 cost</t>
+  </si>
+  <si>
+    <t>Stage 3 effect</t>
+  </si>
+  <si>
+    <t>Stage 4 cost</t>
+  </si>
+  <si>
+    <t>Stage 4 effect</t>
+  </si>
+  <si>
+    <t>OO</t>
+  </si>
+  <si>
+    <t>GG</t>
+  </si>
+  <si>
+    <t>17V</t>
+  </si>
+  <si>
+    <t>Alexandria (B)</t>
+  </si>
+  <si>
+    <t>Babylon (A)</t>
+  </si>
+  <si>
+    <t>Babylon (B)</t>
+  </si>
+  <si>
+    <t>Ephesos (A)</t>
+  </si>
+  <si>
+    <t>Ephesos (B)</t>
+  </si>
+  <si>
+    <t>Giza (A)</t>
+  </si>
+  <si>
+    <t>Giza (B)</t>
+  </si>
+  <si>
+    <t>Halikarnassos (A)</t>
+  </si>
+  <si>
+    <t>Halikarnassos (B)</t>
+  </si>
+  <si>
+    <t>Olympia (A)</t>
+  </si>
+  <si>
+    <t>Olympia (B)</t>
+  </si>
+  <si>
+    <t>Rhodos (A)</t>
+  </si>
+  <si>
+    <t>Rhodos (B)</t>
+  </si>
+  <si>
+    <t>BB</t>
+  </si>
+  <si>
+    <t>4WTOB</t>
+  </si>
+  <si>
+    <t>WW</t>
+  </si>
+  <si>
+    <t>4GLP</t>
+  </si>
+  <si>
+    <t>TTT</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>Wonder name</t>
+  </si>
+  <si>
+    <t>LB</t>
+  </si>
+  <si>
+    <t>WWW</t>
+  </si>
+  <si>
+    <t>6_132</t>
+  </si>
+  <si>
+    <t>BBBB</t>
+  </si>
+  <si>
+    <t>GWW</t>
+  </si>
+  <si>
+    <t>7BB</t>
+  </si>
+  <si>
+    <t>BBBP</t>
+  </si>
+  <si>
+    <t>19$</t>
+  </si>
+  <si>
+    <t>PP</t>
+  </si>
+  <si>
+    <t>LL</t>
+  </si>
+  <si>
+    <t>7EB24</t>
+  </si>
+  <si>
+    <t>7EB54</t>
+  </si>
+  <si>
+    <t>GLP</t>
+  </si>
+  <si>
+    <t>7EB34</t>
+  </si>
+  <si>
+    <t>15V</t>
+  </si>
+  <si>
+    <t>TTTT</t>
+  </si>
+  <si>
+    <t>OOOO</t>
+  </si>
+  <si>
+    <t>OOO</t>
+  </si>
+  <si>
+    <t>BBB</t>
+  </si>
+  <si>
+    <t>PTTTT</t>
+  </si>
+  <si>
+    <t>7HA0</t>
+  </si>
+  <si>
+    <t>7HA2</t>
+  </si>
+  <si>
+    <t>7HA1</t>
+  </si>
+  <si>
+    <t>7OA</t>
+  </si>
+  <si>
+    <t>3BR</t>
+  </si>
+  <si>
+    <t>LOO</t>
+  </si>
+  <si>
+    <t>7OB</t>
+  </si>
+  <si>
+    <t>12S</t>
+  </si>
+  <si>
+    <t>7RB133</t>
+  </si>
+  <si>
+    <t>1RB144</t>
   </si>
 </sst>
 </file>
@@ -1173,8 +1369,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E69" sqref="E69"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A77" sqref="A77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1209,10 +1405,10 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E1" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="F1" t="s">
         <v>96</v>
@@ -1230,7 +1426,7 @@
         <v>100</v>
       </c>
       <c r="K1" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="L1" t="s">
         <v>20</v>
@@ -1245,7 +1441,7 @@
         <v>23</v>
       </c>
       <c r="P1" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="Q1" t="s">
         <v>24</v>
@@ -1260,34 +1456,34 @@
         <v>64</v>
       </c>
       <c r="U1" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="V1" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="W1" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="X1" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="Y1" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="Z1" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="AA1" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="AB1" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="AC1" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="AD1" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.25">
@@ -1298,13 +1494,13 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="D2" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="E2" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -1321,14 +1517,14 @@
       <c r="J2">
         <v>2</v>
       </c>
-      <c r="U2">
-        <v>1</v>
+      <c r="U2" t="s">
+        <v>270</v>
       </c>
       <c r="V2">
         <v>1</v>
       </c>
       <c r="W2" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.25">
@@ -1339,13 +1535,13 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="D3" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="E3" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -1362,14 +1558,14 @@
       <c r="J3">
         <v>2</v>
       </c>
-      <c r="U3">
-        <v>1</v>
+      <c r="U3" t="s">
+        <v>270</v>
       </c>
       <c r="V3">
         <v>1</v>
       </c>
       <c r="W3" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.25">
@@ -1380,13 +1576,13 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="D4" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="E4" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -1403,14 +1599,14 @@
       <c r="J4">
         <v>2</v>
       </c>
-      <c r="U4">
-        <v>1</v>
+      <c r="U4" t="s">
+        <v>270</v>
       </c>
       <c r="V4">
         <v>1</v>
       </c>
       <c r="W4" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.25">
@@ -1421,13 +1617,13 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="D5" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="E5" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -1444,14 +1640,14 @@
       <c r="J5">
         <v>2</v>
       </c>
-      <c r="U5">
-        <v>1</v>
+      <c r="U5" t="s">
+        <v>270</v>
       </c>
       <c r="V5">
         <v>1</v>
       </c>
       <c r="W5" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
@@ -1462,13 +1658,13 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="D6" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="E6" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -1488,11 +1684,11 @@
       <c r="K6">
         <v>1</v>
       </c>
-      <c r="U6">
-        <v>4</v>
+      <c r="U6" t="s">
+        <v>271</v>
       </c>
       <c r="Z6" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.25">
@@ -1503,13 +1699,13 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="D7" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="E7" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -1529,11 +1725,11 @@
       <c r="K7">
         <v>1</v>
       </c>
-      <c r="U7">
-        <v>4</v>
+      <c r="U7" t="s">
+        <v>271</v>
       </c>
       <c r="Z7" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.25">
@@ -1544,13 +1740,13 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="D8" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="E8" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -1570,11 +1766,11 @@
       <c r="K8">
         <v>1</v>
       </c>
-      <c r="U8">
-        <v>4</v>
+      <c r="U8" t="s">
+        <v>271</v>
       </c>
       <c r="Z8" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.25">
@@ -1585,13 +1781,13 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="D9" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="E9" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="F9">
         <v>1</v>
@@ -1611,11 +1807,11 @@
       <c r="K9">
         <v>1</v>
       </c>
-      <c r="U9">
-        <v>4</v>
+      <c r="U9" t="s">
+        <v>271</v>
       </c>
       <c r="Z9" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.25">
@@ -1626,13 +1822,13 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="D10" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="E10" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -1652,11 +1848,11 @@
       <c r="K10">
         <v>1</v>
       </c>
-      <c r="U10">
-        <v>4</v>
+      <c r="U10" t="s">
+        <v>271</v>
       </c>
       <c r="Z10" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.25">
@@ -1667,13 +1863,13 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="D11" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="E11" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -1693,11 +1889,11 @@
       <c r="K11">
         <v>1</v>
       </c>
-      <c r="U11">
-        <v>4</v>
+      <c r="U11" t="s">
+        <v>271</v>
       </c>
       <c r="Z11" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.25">
@@ -1708,13 +1904,13 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="D12" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="E12" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="F12">
         <v>1</v>
@@ -1731,14 +1927,14 @@
       <c r="J12">
         <v>2</v>
       </c>
-      <c r="U12">
-        <v>1</v>
+      <c r="U12" t="s">
+        <v>270</v>
       </c>
       <c r="V12">
         <v>1</v>
       </c>
       <c r="W12" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.25">
@@ -1749,13 +1945,13 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="D13" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="E13" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="F13">
         <v>1</v>
@@ -1772,14 +1968,14 @@
       <c r="J13">
         <v>2</v>
       </c>
-      <c r="U13">
-        <v>1</v>
+      <c r="U13" t="s">
+        <v>270</v>
       </c>
       <c r="V13">
         <v>1</v>
       </c>
       <c r="W13" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.25">
@@ -1790,13 +1986,13 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="D14" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="E14" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="F14">
         <v>1</v>
@@ -1813,14 +2009,14 @@
       <c r="J14">
         <v>2</v>
       </c>
-      <c r="U14">
-        <v>1</v>
+      <c r="U14" t="s">
+        <v>270</v>
       </c>
       <c r="V14">
         <v>1</v>
       </c>
       <c r="W14" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.25">
@@ -1831,10 +2027,10 @@
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="E15" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="F15">
         <v>0</v>
@@ -1851,14 +2047,14 @@
       <c r="J15">
         <v>2</v>
       </c>
-      <c r="U15">
-        <v>1</v>
+      <c r="U15" t="s">
+        <v>270</v>
       </c>
       <c r="V15">
         <v>3</v>
       </c>
       <c r="W15" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.25">
@@ -1869,10 +2065,10 @@
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="E16" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="F16">
         <v>1</v>
@@ -1895,14 +2091,14 @@
       <c r="S16" t="s">
         <v>42</v>
       </c>
-      <c r="U16">
-        <v>1</v>
+      <c r="U16" t="s">
+        <v>270</v>
       </c>
       <c r="V16">
         <v>3</v>
       </c>
       <c r="W16" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.25">
@@ -1913,10 +2109,10 @@
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="E17" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="F17">
         <v>1</v>
@@ -1936,14 +2132,14 @@
       <c r="S17" t="s">
         <v>43</v>
       </c>
-      <c r="U17">
-        <v>1</v>
+      <c r="U17" t="s">
+        <v>270</v>
       </c>
       <c r="V17">
         <v>2</v>
       </c>
       <c r="W17" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.25">
@@ -1954,10 +2150,10 @@
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="E18" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="F18">
         <v>1</v>
@@ -1977,14 +2173,14 @@
       <c r="S18" t="s">
         <v>44</v>
       </c>
-      <c r="U18">
-        <v>1</v>
+      <c r="U18" t="s">
+        <v>270</v>
       </c>
       <c r="V18">
         <v>2</v>
       </c>
       <c r="W18" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.25">
@@ -1998,7 +2194,7 @@
         <v>29</v>
       </c>
       <c r="D19" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="F19">
         <v>0</v>
@@ -2015,14 +2211,14 @@
       <c r="J19">
         <v>3</v>
       </c>
-      <c r="U19">
-        <v>1</v>
+      <c r="U19" t="s">
+        <v>270</v>
       </c>
       <c r="V19">
         <v>1</v>
       </c>
       <c r="W19" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.25">
@@ -2036,10 +2232,10 @@
         <v>29</v>
       </c>
       <c r="D20" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="E20" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="F20">
         <v>1</v>
@@ -2059,11 +2255,11 @@
       <c r="S20" t="s">
         <v>46</v>
       </c>
-      <c r="U20">
-        <v>3</v>
+      <c r="U20" t="s">
+        <v>29</v>
       </c>
       <c r="Y20" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.25">
@@ -2077,10 +2273,10 @@
         <v>29</v>
       </c>
       <c r="D21" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E21" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="F21">
         <v>1</v>
@@ -2100,11 +2296,11 @@
       <c r="S21" t="s">
         <v>46</v>
       </c>
-      <c r="U21">
-        <v>3</v>
+      <c r="U21" t="s">
+        <v>29</v>
       </c>
       <c r="Y21" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.25">
@@ -2118,10 +2314,10 @@
         <v>29</v>
       </c>
       <c r="D22" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="E22" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="F22">
         <v>1</v>
@@ -2141,11 +2337,11 @@
       <c r="S22" t="s">
         <v>47</v>
       </c>
-      <c r="U22">
-        <v>3</v>
+      <c r="U22" t="s">
+        <v>29</v>
       </c>
       <c r="Y22" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.25">
@@ -2159,7 +2355,7 @@
         <v>33</v>
       </c>
       <c r="E23" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="F23">
         <v>1</v>
@@ -2179,14 +2375,14 @@
       <c r="L23">
         <v>1</v>
       </c>
-      <c r="U23">
-        <v>1</v>
+      <c r="U23" t="s">
+        <v>270</v>
       </c>
       <c r="V23">
         <v>1</v>
       </c>
       <c r="W23" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.25">
@@ -2200,7 +2396,7 @@
         <v>33</v>
       </c>
       <c r="E24" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="F24">
         <v>1</v>
@@ -2220,14 +2416,14 @@
       <c r="O24">
         <v>1</v>
       </c>
-      <c r="U24">
-        <v>1</v>
+      <c r="U24" t="s">
+        <v>270</v>
       </c>
       <c r="V24">
         <v>1</v>
       </c>
       <c r="W24" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.25">
@@ -2241,7 +2437,7 @@
         <v>33</v>
       </c>
       <c r="E25" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="F25">
         <v>1</v>
@@ -2261,14 +2457,14 @@
       <c r="N25">
         <v>1</v>
       </c>
-      <c r="U25">
-        <v>1</v>
+      <c r="U25" t="s">
+        <v>270</v>
       </c>
       <c r="V25">
         <v>1</v>
       </c>
       <c r="W25" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.25">
@@ -2282,7 +2478,7 @@
         <v>36</v>
       </c>
       <c r="E26" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="F26">
         <v>1</v>
@@ -2308,11 +2504,11 @@
       <c r="T26" t="s">
         <v>54</v>
       </c>
-      <c r="U26">
-        <v>2</v>
+      <c r="U26" t="s">
+        <v>36</v>
       </c>
       <c r="X26" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.25">
@@ -2326,7 +2522,7 @@
         <v>36</v>
       </c>
       <c r="E27" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="F27">
         <v>1</v>
@@ -2352,11 +2548,11 @@
       <c r="T27" t="s">
         <v>55</v>
       </c>
-      <c r="U27">
-        <v>2</v>
+      <c r="U27" t="s">
+        <v>36</v>
       </c>
       <c r="X27" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.25">
@@ -2370,7 +2566,7 @@
         <v>36</v>
       </c>
       <c r="E28" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="F28">
         <v>1</v>
@@ -2396,11 +2592,11 @@
       <c r="T28" t="s">
         <v>56</v>
       </c>
-      <c r="U28">
-        <v>2</v>
+      <c r="U28" t="s">
+        <v>36</v>
       </c>
       <c r="X28" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.25">
@@ -2411,13 +2607,13 @@
         <v>2</v>
       </c>
       <c r="C29" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="D29" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="E29" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="F29">
         <v>1</v>
@@ -2437,14 +2633,14 @@
       <c r="K29">
         <v>1</v>
       </c>
-      <c r="U29">
-        <v>1</v>
+      <c r="U29" t="s">
+        <v>270</v>
       </c>
       <c r="V29">
         <v>2</v>
       </c>
       <c r="W29" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.25">
@@ -2455,13 +2651,13 @@
         <v>2</v>
       </c>
       <c r="C30" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="D30" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="E30" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="F30">
         <v>1</v>
@@ -2481,14 +2677,14 @@
       <c r="K30">
         <v>1</v>
       </c>
-      <c r="U30">
-        <v>1</v>
+      <c r="U30" t="s">
+        <v>270</v>
       </c>
       <c r="V30">
         <v>2</v>
       </c>
       <c r="W30" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.25">
@@ -2499,13 +2695,13 @@
         <v>2</v>
       </c>
       <c r="C31" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="D31" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="E31" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="F31">
         <v>1</v>
@@ -2525,14 +2721,14 @@
       <c r="K31">
         <v>1</v>
       </c>
-      <c r="U31">
-        <v>1</v>
+      <c r="U31" t="s">
+        <v>270</v>
       </c>
       <c r="V31">
         <v>2</v>
       </c>
       <c r="W31" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.25">
@@ -2543,13 +2739,13 @@
         <v>2</v>
       </c>
       <c r="C32" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="D32" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="E32" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="F32">
         <v>1</v>
@@ -2569,14 +2765,14 @@
       <c r="K32">
         <v>1</v>
       </c>
-      <c r="U32">
-        <v>1</v>
+      <c r="U32" t="s">
+        <v>270</v>
       </c>
       <c r="V32">
         <v>2</v>
       </c>
       <c r="W32" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
     </row>
     <row r="33" spans="1:30" x14ac:dyDescent="0.25">
@@ -2587,13 +2783,13 @@
         <v>2</v>
       </c>
       <c r="C33" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="D33" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="E33" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="F33">
         <v>1</v>
@@ -2610,14 +2806,14 @@
       <c r="J33">
         <v>2</v>
       </c>
-      <c r="U33">
-        <v>1</v>
+      <c r="U33" t="s">
+        <v>270</v>
       </c>
       <c r="V33">
         <v>1</v>
       </c>
       <c r="W33" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
     </row>
     <row r="34" spans="1:30" x14ac:dyDescent="0.25">
@@ -2628,13 +2824,13 @@
         <v>2</v>
       </c>
       <c r="C34" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="D34" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="E34" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="F34">
         <v>1</v>
@@ -2651,14 +2847,14 @@
       <c r="J34">
         <v>2</v>
       </c>
-      <c r="U34">
-        <v>1</v>
+      <c r="U34" t="s">
+        <v>270</v>
       </c>
       <c r="V34">
         <v>1</v>
       </c>
       <c r="W34" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
     </row>
     <row r="35" spans="1:30" x14ac:dyDescent="0.25">
@@ -2669,13 +2865,13 @@
         <v>2</v>
       </c>
       <c r="C35" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="D35" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="E35" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="F35">
         <v>1</v>
@@ -2692,14 +2888,14 @@
       <c r="J35">
         <v>2</v>
       </c>
-      <c r="U35">
-        <v>1</v>
+      <c r="U35" t="s">
+        <v>270</v>
       </c>
       <c r="V35">
         <v>1</v>
       </c>
       <c r="W35" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
     </row>
     <row r="36" spans="1:30" x14ac:dyDescent="0.25">
@@ -2710,10 +2906,10 @@
         <v>2</v>
       </c>
       <c r="C36" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="E36" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="F36">
         <v>1</v>
@@ -2733,14 +2929,14 @@
       <c r="M36">
         <v>3</v>
       </c>
-      <c r="U36">
-        <v>1</v>
+      <c r="U36" t="s">
+        <v>270</v>
       </c>
       <c r="V36">
         <v>5</v>
       </c>
       <c r="W36" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="37" spans="1:30" x14ac:dyDescent="0.25">
@@ -2751,10 +2947,10 @@
         <v>2</v>
       </c>
       <c r="C37" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="E37" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="F37">
         <v>1</v>
@@ -2783,14 +2979,14 @@
       <c r="S37" t="s">
         <v>58</v>
       </c>
-      <c r="U37">
-        <v>1</v>
+      <c r="U37" t="s">
+        <v>270</v>
       </c>
       <c r="V37">
         <v>3</v>
       </c>
       <c r="W37" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="38" spans="1:30" x14ac:dyDescent="0.25">
@@ -2801,10 +2997,10 @@
         <v>2</v>
       </c>
       <c r="C38" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="E38" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="F38">
         <v>1</v>
@@ -2830,14 +3026,14 @@
       <c r="S38" t="s">
         <v>59</v>
       </c>
-      <c r="U38">
-        <v>1</v>
+      <c r="U38" t="s">
+        <v>270</v>
       </c>
       <c r="V38">
         <v>4</v>
       </c>
       <c r="W38" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="39" spans="1:30" x14ac:dyDescent="0.25">
@@ -2848,10 +3044,10 @@
         <v>2</v>
       </c>
       <c r="C39" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="E39" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="F39">
         <v>1</v>
@@ -2874,14 +3070,14 @@
       <c r="P39">
         <v>1</v>
       </c>
-      <c r="U39">
-        <v>1</v>
+      <c r="U39" t="s">
+        <v>270</v>
       </c>
       <c r="V39">
         <v>4</v>
       </c>
       <c r="W39" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="40" spans="1:30" x14ac:dyDescent="0.25">
@@ -2895,10 +3091,10 @@
         <v>29</v>
       </c>
       <c r="D40" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="E40" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="F40">
         <v>1</v>
@@ -2921,11 +3117,11 @@
       <c r="S40" t="s">
         <v>65</v>
       </c>
-      <c r="U40">
-        <v>4</v>
+      <c r="U40" t="s">
+        <v>271</v>
       </c>
       <c r="Z40" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="41" spans="1:30" x14ac:dyDescent="0.25">
@@ -2939,10 +3135,10 @@
         <v>29</v>
       </c>
       <c r="D41" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="E41" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="F41">
         <v>1</v>
@@ -2965,11 +3161,11 @@
       <c r="S41" t="s">
         <v>66</v>
       </c>
-      <c r="U41">
-        <v>4</v>
+      <c r="U41" t="s">
+        <v>271</v>
       </c>
       <c r="Z41" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
     </row>
     <row r="42" spans="1:30" x14ac:dyDescent="0.25">
@@ -2983,7 +3179,7 @@
         <v>29</v>
       </c>
       <c r="D42" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="F42">
         <v>1</v>
@@ -3000,14 +3196,14 @@
       <c r="J42">
         <v>3</v>
       </c>
-      <c r="U42">
-        <v>5</v>
+      <c r="U42" t="s">
+        <v>272</v>
       </c>
       <c r="AA42" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="AB42" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="AC42">
         <v>1</v>
@@ -3027,7 +3223,7 @@
         <v>29</v>
       </c>
       <c r="D43" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="F43">
         <v>0</v>
@@ -3044,14 +3240,14 @@
       <c r="J43">
         <v>2</v>
       </c>
-      <c r="U43">
-        <v>5</v>
+      <c r="U43" t="s">
+        <v>272</v>
       </c>
       <c r="AA43" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="AB43" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="AC43">
         <v>2</v>
@@ -3071,7 +3267,7 @@
         <v>33</v>
       </c>
       <c r="E44" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="F44">
         <v>1</v>
@@ -3094,14 +3290,14 @@
       <c r="S44" t="s">
         <v>69</v>
       </c>
-      <c r="U44">
-        <v>1</v>
+      <c r="U44" t="s">
+        <v>270</v>
       </c>
       <c r="V44">
         <v>2</v>
       </c>
       <c r="W44" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="45" spans="1:30" x14ac:dyDescent="0.25">
@@ -3115,7 +3311,7 @@
         <v>33</v>
       </c>
       <c r="E45" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="F45">
         <v>0</v>
@@ -3141,14 +3337,14 @@
       <c r="S45" t="s">
         <v>70</v>
       </c>
-      <c r="U45">
-        <v>1</v>
+      <c r="U45" t="s">
+        <v>270</v>
       </c>
       <c r="V45">
         <v>2</v>
       </c>
       <c r="W45" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="46" spans="1:30" x14ac:dyDescent="0.25">
@@ -3162,7 +3358,7 @@
         <v>33</v>
       </c>
       <c r="E46" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="F46">
         <v>1</v>
@@ -3188,14 +3384,14 @@
       <c r="O46">
         <v>1</v>
       </c>
-      <c r="U46">
-        <v>1</v>
+      <c r="U46" t="s">
+        <v>270</v>
       </c>
       <c r="V46">
         <v>2</v>
       </c>
       <c r="W46" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="47" spans="1:30" x14ac:dyDescent="0.25">
@@ -3209,7 +3405,7 @@
         <v>33</v>
       </c>
       <c r="E47" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="F47">
         <v>1</v>
@@ -3232,14 +3428,14 @@
       <c r="O47">
         <v>1</v>
       </c>
-      <c r="U47">
-        <v>1</v>
+      <c r="U47" t="s">
+        <v>270</v>
       </c>
       <c r="V47">
         <v>2</v>
       </c>
       <c r="W47" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="48" spans="1:30" x14ac:dyDescent="0.25">
@@ -3253,7 +3449,7 @@
         <v>36</v>
       </c>
       <c r="E48" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="F48">
         <v>1</v>
@@ -3282,11 +3478,11 @@
       <c r="T48" t="s">
         <v>73</v>
       </c>
-      <c r="U48">
-        <v>2</v>
+      <c r="U48" t="s">
+        <v>36</v>
       </c>
       <c r="X48" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
     </row>
     <row r="49" spans="1:30" x14ac:dyDescent="0.25">
@@ -3300,7 +3496,7 @@
         <v>36</v>
       </c>
       <c r="E49" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="F49">
         <v>1</v>
@@ -3329,11 +3525,11 @@
       <c r="T49" t="s">
         <v>74</v>
       </c>
-      <c r="U49">
-        <v>2</v>
+      <c r="U49" t="s">
+        <v>36</v>
       </c>
       <c r="X49" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
     </row>
     <row r="50" spans="1:30" x14ac:dyDescent="0.25">
@@ -3347,7 +3543,7 @@
         <v>36</v>
       </c>
       <c r="E50" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="F50">
         <v>1</v>
@@ -3376,11 +3572,11 @@
       <c r="T50" t="s">
         <v>75</v>
       </c>
-      <c r="U50">
-        <v>2</v>
+      <c r="U50" t="s">
+        <v>36</v>
       </c>
       <c r="X50" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
     </row>
     <row r="51" spans="1:30" x14ac:dyDescent="0.25">
@@ -3394,7 +3590,7 @@
         <v>36</v>
       </c>
       <c r="E51" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="F51">
         <v>1</v>
@@ -3423,11 +3619,11 @@
       <c r="T51" t="s">
         <v>77</v>
       </c>
-      <c r="U51">
-        <v>2</v>
+      <c r="U51" t="s">
+        <v>36</v>
       </c>
       <c r="X51" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
     </row>
     <row r="52" spans="1:30" x14ac:dyDescent="0.25">
@@ -3438,10 +3634,10 @@
         <v>3</v>
       </c>
       <c r="C52" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="E52" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="F52">
         <v>1</v>
@@ -3473,14 +3669,14 @@
       <c r="R52">
         <v>1</v>
       </c>
-      <c r="U52">
-        <v>1</v>
+      <c r="U52" t="s">
+        <v>270</v>
       </c>
       <c r="V52">
         <v>7</v>
       </c>
       <c r="W52" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="53" spans="1:30" x14ac:dyDescent="0.25">
@@ -3491,10 +3687,10 @@
         <v>3</v>
       </c>
       <c r="C53" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="E53" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="F53">
         <v>1</v>
@@ -3517,14 +3713,14 @@
       <c r="N53">
         <v>2</v>
       </c>
-      <c r="U53">
-        <v>1</v>
+      <c r="U53" t="s">
+        <v>270</v>
       </c>
       <c r="V53">
         <v>5</v>
       </c>
       <c r="W53" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="54" spans="1:30" x14ac:dyDescent="0.25">
@@ -3535,10 +3731,10 @@
         <v>3</v>
       </c>
       <c r="C54" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="E54" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="F54">
         <v>1</v>
@@ -3564,14 +3760,14 @@
       <c r="Q54">
         <v>1</v>
       </c>
-      <c r="U54">
-        <v>1</v>
+      <c r="U54" t="s">
+        <v>270</v>
       </c>
       <c r="V54">
         <v>6</v>
       </c>
       <c r="W54" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="55" spans="1:30" x14ac:dyDescent="0.25">
@@ -3582,10 +3778,10 @@
         <v>3</v>
       </c>
       <c r="C55" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="E55" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="F55">
         <v>1</v>
@@ -3623,14 +3819,14 @@
       <c r="R55">
         <v>1</v>
       </c>
-      <c r="U55">
-        <v>1</v>
+      <c r="U55" t="s">
+        <v>270</v>
       </c>
       <c r="V55">
         <v>8</v>
       </c>
       <c r="W55" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="56" spans="1:30" x14ac:dyDescent="0.25">
@@ -3641,10 +3837,10 @@
         <v>3</v>
       </c>
       <c r="C56" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="E56" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="F56">
         <v>1</v>
@@ -3670,14 +3866,14 @@
       <c r="O56">
         <v>1</v>
       </c>
-      <c r="U56">
-        <v>1</v>
+      <c r="U56" t="s">
+        <v>270</v>
       </c>
       <c r="V56">
         <v>6</v>
       </c>
       <c r="W56" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="57" spans="1:30" x14ac:dyDescent="0.25">
@@ -3691,7 +3887,7 @@
         <v>29</v>
       </c>
       <c r="D57" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="F57">
         <v>1</v>
@@ -3717,14 +3913,14 @@
       <c r="P57">
         <v>1</v>
       </c>
-      <c r="U57">
-        <v>5</v>
+      <c r="U57" t="s">
+        <v>272</v>
       </c>
       <c r="AA57" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="AB57" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="AC57">
         <v>1</v>
@@ -3744,7 +3940,7 @@
         <v>29</v>
       </c>
       <c r="D58" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="F58">
         <v>1</v>
@@ -3767,11 +3963,11 @@
       <c r="Q58">
         <v>1</v>
       </c>
-      <c r="U58">
-        <v>5</v>
+      <c r="U58" t="s">
+        <v>272</v>
       </c>
       <c r="AA58" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="AB58" t="s">
         <v>29</v>
@@ -3794,7 +3990,7 @@
         <v>29</v>
       </c>
       <c r="D59" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="F59">
         <v>0</v>
@@ -3817,14 +4013,14 @@
       <c r="R59">
         <v>1</v>
       </c>
-      <c r="U59">
-        <v>5</v>
+      <c r="U59" t="s">
+        <v>272</v>
       </c>
       <c r="AA59" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="AB59" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="AC59">
         <v>2</v>
@@ -3844,7 +4040,7 @@
         <v>29</v>
       </c>
       <c r="D60" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="F60">
         <v>1</v>
@@ -3867,14 +4063,14 @@
       <c r="O60">
         <v>1</v>
       </c>
-      <c r="U60">
-        <v>5</v>
+      <c r="U60" t="s">
+        <v>272</v>
       </c>
       <c r="AA60" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="AB60" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="AC60">
         <v>3</v>
@@ -3894,7 +4090,7 @@
         <v>33</v>
       </c>
       <c r="E61" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="F61">
         <v>1</v>
@@ -3917,14 +4113,14 @@
       <c r="O61">
         <v>3</v>
       </c>
-      <c r="U61">
-        <v>1</v>
+      <c r="U61" t="s">
+        <v>270</v>
       </c>
       <c r="V61">
         <v>3</v>
       </c>
       <c r="W61" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="62" spans="1:30" x14ac:dyDescent="0.25">
@@ -3938,7 +4134,7 @@
         <v>33</v>
       </c>
       <c r="E62" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="F62">
         <v>0</v>
@@ -3961,14 +4157,14 @@
       <c r="O62">
         <v>1</v>
       </c>
-      <c r="U62">
-        <v>1</v>
+      <c r="U62" t="s">
+        <v>270</v>
       </c>
       <c r="V62">
         <v>3</v>
       </c>
       <c r="W62" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="63" spans="1:30" x14ac:dyDescent="0.25">
@@ -3982,7 +4178,7 @@
         <v>33</v>
       </c>
       <c r="E63" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="F63">
         <v>1</v>
@@ -4008,14 +4204,14 @@
       <c r="P63">
         <v>1</v>
       </c>
-      <c r="U63">
-        <v>1</v>
+      <c r="U63" t="s">
+        <v>270</v>
       </c>
       <c r="V63">
         <v>3</v>
       </c>
       <c r="W63" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="64" spans="1:30" x14ac:dyDescent="0.25">
@@ -4029,7 +4225,7 @@
         <v>33</v>
       </c>
       <c r="E64" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="F64">
         <v>1</v>
@@ -4052,14 +4248,14 @@
       <c r="N64">
         <v>3</v>
       </c>
-      <c r="U64">
-        <v>1</v>
+      <c r="U64" t="s">
+        <v>270</v>
       </c>
       <c r="V64">
         <v>3</v>
       </c>
       <c r="W64" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="65" spans="1:30" x14ac:dyDescent="0.25">
@@ -4073,7 +4269,7 @@
         <v>36</v>
       </c>
       <c r="E65" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="F65">
         <v>1</v>
@@ -4099,11 +4295,11 @@
       <c r="R65">
         <v>1</v>
       </c>
-      <c r="U65">
-        <v>2</v>
+      <c r="U65" t="s">
+        <v>36</v>
       </c>
       <c r="X65" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
     </row>
     <row r="66" spans="1:30" x14ac:dyDescent="0.25">
@@ -4117,7 +4313,7 @@
         <v>36</v>
       </c>
       <c r="E66" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="F66">
         <v>1</v>
@@ -4143,11 +4339,11 @@
       <c r="Q66">
         <v>1</v>
       </c>
-      <c r="U66">
-        <v>2</v>
+      <c r="U66" t="s">
+        <v>36</v>
       </c>
       <c r="X66" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
     </row>
     <row r="67" spans="1:30" x14ac:dyDescent="0.25">
@@ -4161,7 +4357,7 @@
         <v>36</v>
       </c>
       <c r="E67" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="F67">
         <v>1</v>
@@ -4187,11 +4383,11 @@
       <c r="R67">
         <v>1</v>
       </c>
-      <c r="U67">
-        <v>2</v>
+      <c r="U67" t="s">
+        <v>36</v>
       </c>
       <c r="X67" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
     </row>
     <row r="68" spans="1:30" x14ac:dyDescent="0.25">
@@ -4205,7 +4401,7 @@
         <v>36</v>
       </c>
       <c r="E68" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="F68">
         <v>1</v>
@@ -4228,11 +4424,11 @@
       <c r="Q68">
         <v>1</v>
       </c>
-      <c r="U68">
-        <v>2</v>
+      <c r="U68" t="s">
+        <v>36</v>
       </c>
       <c r="X68" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
     </row>
     <row r="69" spans="1:30" x14ac:dyDescent="0.25">
@@ -4246,7 +4442,7 @@
         <v>36</v>
       </c>
       <c r="E69" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="F69">
         <v>1</v>
@@ -4272,11 +4468,11 @@
       <c r="R69">
         <v>1</v>
       </c>
-      <c r="U69">
-        <v>2</v>
+      <c r="U69" t="s">
+        <v>36</v>
       </c>
       <c r="X69" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
     </row>
     <row r="70" spans="1:30" x14ac:dyDescent="0.25">
@@ -4319,14 +4515,14 @@
       <c r="O70">
         <v>2</v>
       </c>
-      <c r="U70">
-        <v>5</v>
+      <c r="U70" t="s">
+        <v>272</v>
       </c>
       <c r="AA70" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="AB70" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="AC70">
         <v>0</v>
@@ -4369,14 +4565,14 @@
       <c r="O71">
         <v>2</v>
       </c>
-      <c r="U71">
-        <v>5</v>
+      <c r="U71" t="s">
+        <v>272</v>
       </c>
       <c r="AA71" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="AB71" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="AC71">
         <v>0</v>
@@ -4422,11 +4618,11 @@
       <c r="R72">
         <v>1</v>
       </c>
-      <c r="U72">
-        <v>5</v>
+      <c r="U72" t="s">
+        <v>272</v>
       </c>
       <c r="AA72" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="AB72" t="s">
         <v>29</v>
@@ -4475,11 +4671,11 @@
       <c r="R73">
         <v>1</v>
       </c>
-      <c r="U73">
-        <v>5</v>
+      <c r="U73" t="s">
+        <v>272</v>
       </c>
       <c r="AA73" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="AB73" t="s">
         <v>36</v>
@@ -4525,14 +4721,14 @@
       <c r="Q74">
         <v>1</v>
       </c>
-      <c r="U74">
-        <v>5</v>
+      <c r="U74" t="s">
+        <v>272</v>
       </c>
       <c r="AA74" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="AB74" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="AC74">
         <v>0</v>
@@ -4578,14 +4774,14 @@
       <c r="P75">
         <v>1</v>
       </c>
-      <c r="U75">
-        <v>5</v>
+      <c r="U75" t="s">
+        <v>272</v>
       </c>
       <c r="AA75" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="AB75" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="AC75">
         <v>0</v>
@@ -4605,7 +4801,7 @@
         <v>78</v>
       </c>
       <c r="D76" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="F76">
         <v>1</v>
@@ -4631,8 +4827,8 @@
       <c r="R76">
         <v>1</v>
       </c>
-      <c r="U76">
-        <v>6</v>
+      <c r="U76" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="77" spans="1:30" x14ac:dyDescent="0.25">
@@ -4646,7 +4842,7 @@
         <v>78</v>
       </c>
       <c r="D77" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="F77">
         <v>1</v>
@@ -4672,8 +4868,8 @@
       <c r="R77">
         <v>1</v>
       </c>
-      <c r="U77">
-        <v>6</v>
+      <c r="U77" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="78" spans="1:30" x14ac:dyDescent="0.25">
@@ -4687,7 +4883,7 @@
         <v>78</v>
       </c>
       <c r="D78" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="F78">
         <v>1</v>
@@ -4713,14 +4909,14 @@
       <c r="R78">
         <v>1</v>
       </c>
-      <c r="U78">
-        <v>5</v>
+      <c r="U78" t="s">
+        <v>272</v>
       </c>
       <c r="AA78" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="AB78" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="AC78">
         <v>0</v>
@@ -4740,7 +4936,7 @@
         <v>78</v>
       </c>
       <c r="D79" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="F79">
         <v>1</v>
@@ -4766,14 +4962,14 @@
       <c r="Q79">
         <v>1</v>
       </c>
-      <c r="U79">
-        <v>5</v>
+      <c r="U79" t="s">
+        <v>272</v>
       </c>
       <c r="AA79" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="AB79" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="AC79">
         <v>0</v>
@@ -4790,16 +4986,483 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>309</v>
+      </c>
+      <c r="B1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C1" t="s">
+        <v>275</v>
+      </c>
+      <c r="D1" t="s">
+        <v>277</v>
+      </c>
+      <c r="E1" t="s">
+        <v>279</v>
+      </c>
+      <c r="F1" t="s">
+        <v>281</v>
+      </c>
+      <c r="G1" t="s">
+        <v>282</v>
+      </c>
+      <c r="H1" t="s">
+        <v>283</v>
+      </c>
+      <c r="I1" t="s">
+        <v>284</v>
+      </c>
+      <c r="J1" t="s">
+        <v>285</v>
+      </c>
+      <c r="K1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>274</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D2" t="s">
+        <v>278</v>
+      </c>
+      <c r="E2" t="s">
+        <v>280</v>
+      </c>
+      <c r="F2" t="s">
+        <v>287</v>
+      </c>
+      <c r="G2" t="s">
+        <v>304</v>
+      </c>
+      <c r="H2" t="s">
+        <v>288</v>
+      </c>
+      <c r="I2" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>290</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>172</v>
+      </c>
+      <c r="D3" t="s">
+        <v>303</v>
+      </c>
+      <c r="E3" t="s">
+        <v>304</v>
+      </c>
+      <c r="F3" t="s">
+        <v>305</v>
+      </c>
+      <c r="G3" t="s">
+        <v>306</v>
+      </c>
+      <c r="H3" t="s">
+        <v>307</v>
+      </c>
+      <c r="I3" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>291</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>175</v>
+      </c>
+      <c r="D4" t="s">
+        <v>303</v>
+      </c>
+      <c r="E4" t="s">
+        <v>280</v>
+      </c>
+      <c r="F4" t="s">
+        <v>311</v>
+      </c>
+      <c r="G4" t="s">
+        <v>312</v>
+      </c>
+      <c r="H4" t="s">
+        <v>313</v>
+      </c>
+      <c r="I4" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>292</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>175</v>
+      </c>
+      <c r="D5" t="s">
+        <v>310</v>
+      </c>
+      <c r="E5" t="s">
+        <v>280</v>
+      </c>
+      <c r="F5" t="s">
+        <v>314</v>
+      </c>
+      <c r="G5" t="s">
+        <v>315</v>
+      </c>
+      <c r="H5" t="s">
+        <v>316</v>
+      </c>
+      <c r="I5" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>293</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>174</v>
+      </c>
+      <c r="D6" t="s">
+        <v>278</v>
+      </c>
+      <c r="E6" t="s">
+        <v>280</v>
+      </c>
+      <c r="F6" t="s">
+        <v>305</v>
+      </c>
+      <c r="G6" t="s">
+        <v>317</v>
+      </c>
+      <c r="H6" t="s">
+        <v>318</v>
+      </c>
+      <c r="I6" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>294</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>174</v>
+      </c>
+      <c r="D7" t="s">
+        <v>278</v>
+      </c>
+      <c r="E7" t="s">
+        <v>320</v>
+      </c>
+      <c r="F7" t="s">
+        <v>305</v>
+      </c>
+      <c r="G7" t="s">
+        <v>323</v>
+      </c>
+      <c r="H7" t="s">
+        <v>322</v>
+      </c>
+      <c r="I7" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>295</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>171</v>
+      </c>
+      <c r="D8" t="s">
+        <v>278</v>
+      </c>
+      <c r="E8" t="s">
+        <v>280</v>
+      </c>
+      <c r="F8" t="s">
+        <v>311</v>
+      </c>
+      <c r="G8" t="s">
+        <v>324</v>
+      </c>
+      <c r="H8" t="s">
+        <v>325</v>
+      </c>
+      <c r="I8" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>296</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D9" t="s">
+        <v>305</v>
+      </c>
+      <c r="E9" t="s">
+        <v>280</v>
+      </c>
+      <c r="F9" t="s">
+        <v>307</v>
+      </c>
+      <c r="G9" t="s">
+        <v>324</v>
+      </c>
+      <c r="H9" t="s">
+        <v>328</v>
+      </c>
+      <c r="I9" t="s">
+        <v>324</v>
+      </c>
+      <c r="J9" t="s">
+        <v>329</v>
+      </c>
+      <c r="K9" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>297</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>308</v>
+      </c>
+      <c r="D10" t="s">
+        <v>303</v>
+      </c>
+      <c r="E10" t="s">
+        <v>280</v>
+      </c>
+      <c r="F10" t="s">
+        <v>327</v>
+      </c>
+      <c r="G10" t="s">
+        <v>330</v>
+      </c>
+      <c r="H10" t="s">
+        <v>319</v>
+      </c>
+      <c r="I10" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>298</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>308</v>
+      </c>
+      <c r="D11" t="s">
+        <v>287</v>
+      </c>
+      <c r="E11" t="s">
+        <v>331</v>
+      </c>
+      <c r="F11" t="s">
+        <v>328</v>
+      </c>
+      <c r="G11" t="s">
+        <v>332</v>
+      </c>
+      <c r="H11" t="s">
+        <v>322</v>
+      </c>
+      <c r="I11" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>299</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>162</v>
+      </c>
+      <c r="D12" t="s">
+        <v>305</v>
+      </c>
+      <c r="E12" t="s">
+        <v>280</v>
+      </c>
+      <c r="F12" t="s">
+        <v>278</v>
+      </c>
+      <c r="G12" t="s">
+        <v>333</v>
+      </c>
+      <c r="H12" t="s">
+        <v>287</v>
+      </c>
+      <c r="I12" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>300</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
+        <v>162</v>
+      </c>
+      <c r="D13" t="s">
+        <v>305</v>
+      </c>
+      <c r="E13" t="s">
+        <v>334</v>
+      </c>
+      <c r="F13" t="s">
+        <v>278</v>
+      </c>
+      <c r="G13" t="s">
+        <v>324</v>
+      </c>
+      <c r="H13" t="s">
+        <v>335</v>
+      </c>
+      <c r="I13" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>301</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14" t="s">
+        <v>165</v>
+      </c>
+      <c r="D14" t="s">
+        <v>305</v>
+      </c>
+      <c r="E14" t="s">
+        <v>280</v>
+      </c>
+      <c r="F14" t="s">
+        <v>328</v>
+      </c>
+      <c r="G14" t="s">
+        <v>337</v>
+      </c>
+      <c r="H14" t="s">
+        <v>326</v>
+      </c>
+      <c r="I14" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>302</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>165</v>
+      </c>
+      <c r="D15" t="s">
+        <v>307</v>
+      </c>
+      <c r="E15" t="s">
+        <v>338</v>
+      </c>
+      <c r="F15" t="s">
+        <v>326</v>
+      </c>
+      <c r="G15" t="s">
+        <v>339</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="A2" sqref="A2:J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="10" max="10" width="32" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="32" customWidth="1"/>
+    <col min="12" max="12" width="28.85546875" customWidth="1"/>
     <col min="13" max="13" width="71" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4832,57 +5495,27 @@
         <v>107</v>
       </c>
       <c r="J1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="L1" t="s">
+        <v>108</v>
+      </c>
+      <c r="M1" t="s">
+        <v>110</v>
+      </c>
+      <c r="N1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2" t="s">
         <v>112</v>
       </c>
-      <c r="M1" t="s">
-        <v>114</v>
-      </c>
-      <c r="N1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>111</v>
-      </c>
-      <c r="F2" t="s">
-        <v>111</v>
-      </c>
-      <c r="G2" t="s">
-        <v>108</v>
-      </c>
-      <c r="H2" t="s">
-        <v>109</v>
-      </c>
-      <c r="I2" t="s">
-        <v>110</v>
-      </c>
-      <c r="J2" t="s">
-        <v>117</v>
-      </c>
-      <c r="L2">
-        <v>1</v>
-      </c>
-      <c r="M2" t="s">
-        <v>116</v>
-      </c>
       <c r="N2" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -4890,7 +5523,7 @@
         <v>2</v>
       </c>
       <c r="M3" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -4898,10 +5531,10 @@
         <v>3</v>
       </c>
       <c r="M4" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="N4" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -4909,10 +5542,10 @@
         <v>4</v>
       </c>
       <c r="M5" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="N5" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -4920,10 +5553,10 @@
         <v>5</v>
       </c>
       <c r="M6" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="N6" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -4931,10 +5564,10 @@
         <v>6</v>
       </c>
       <c r="M7" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="N7" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -4942,10 +5575,10 @@
         <v>7</v>
       </c>
       <c r="M8" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="N8" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -4953,182 +5586,182 @@
         <v>8</v>
       </c>
       <c r="M9" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="L11" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="L12" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M13" s="1" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M14" s="1" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M15" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M16" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="17" spans="12:13" x14ac:dyDescent="0.25">
       <c r="M17" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="18" spans="12:13" x14ac:dyDescent="0.25">
       <c r="M18" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="19" spans="12:13" x14ac:dyDescent="0.25">
       <c r="M19" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="20" spans="12:13" x14ac:dyDescent="0.25">
       <c r="M20" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="21" spans="12:13" x14ac:dyDescent="0.25">
       <c r="M21" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
     <row r="22" spans="12:13" x14ac:dyDescent="0.25">
       <c r="M22" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="23" spans="12:13" x14ac:dyDescent="0.25">
       <c r="M23" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="24" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L24" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="25" spans="12:13" x14ac:dyDescent="0.25">
       <c r="M25" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
     </row>
     <row r="26" spans="12:13" x14ac:dyDescent="0.25">
       <c r="M26" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
     <row r="27" spans="12:13" x14ac:dyDescent="0.25">
       <c r="M27" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="28" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L28" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="29" spans="12:13" x14ac:dyDescent="0.25">
       <c r="M29" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
     </row>
     <row r="30" spans="12:13" x14ac:dyDescent="0.25">
       <c r="M30" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="31" spans="12:13" x14ac:dyDescent="0.25">
       <c r="M31" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="32" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L32" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
     </row>
     <row r="33" spans="12:13" x14ac:dyDescent="0.25">
       <c r="M33" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="34" spans="12:13" x14ac:dyDescent="0.25">
       <c r="M34" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
     <row r="35" spans="12:13" x14ac:dyDescent="0.25">
       <c r="M35" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="36" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L36" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="37" spans="12:13" x14ac:dyDescent="0.25">
       <c r="M37" s="1" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="38" spans="12:13" x14ac:dyDescent="0.25">
       <c r="M38" s="1" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="39" spans="12:13" x14ac:dyDescent="0.25">
       <c r="M39" s="1" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
     </row>
     <row r="40" spans="12:13" x14ac:dyDescent="0.25">
       <c r="M40" s="1" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
     <row r="41" spans="12:13" x14ac:dyDescent="0.25">
       <c r="M41" s="1" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="42" spans="12:13" x14ac:dyDescent="0.25">
       <c r="M42" s="1" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="45" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L45" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
     </row>
     <row r="46" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L46" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
     </row>
     <row r="47" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L47" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>

</xml_diff>